<commit_message>
I would like to script in roblox studio more bruh
</commit_message>
<xml_diff>
--- a/data/lab05/samples/ex1.xlsx
+++ b/data/lab05/samples/ex1.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,290 +421,172 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="41" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>[</t>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>age</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>city</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>email</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  {</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Анна Иванова</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>anna.ivanova@example.com</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">    "id": "1"</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Дмитрий Петров</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>dmitry.petrov@example.com</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    "name": "Анна Иванова"</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Елена Смирнова</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Казань</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>elena.smirnova@example.com</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">    "age": "28"</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Иван Кузнецов</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Новосибирск</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ivan.kuznetsov@example.com</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">    "city": "Москва"</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "email": "anna.ivanova@example.com"</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  }</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  {</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "id": "2"</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "name": "Дмитрий Петров"</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "age": "35"</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "city": "Санкт-Петербург"</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "email": "dmitry.petrov@example.com"</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  }</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  {</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "id": "3"</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "name": "Елена Смирнова"</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "age": "22"</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "city": "Казань"</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "email": "elena.smirnova@example.com"</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  }</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  {</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "id": "4"</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "name": "Иван Кузнецов"</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "age": "41"</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "city": "Новосибирск"</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "email": "ivan.kuznetsov@example.com"</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  }</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  {</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "id": "5"</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr"/>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "name": "Ольга Соколова"</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr"/>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "age": "30"</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr"/>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "city": "Екатеринбург"</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr"/>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    "email": "olga.sokolova@example.com"</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  }</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>]</t>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Ольга Соколова</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Екатеринбург</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>olga.sokolova@example.com</t>
         </is>
       </c>
     </row>

</xml_diff>